<commit_message>
Subida de Planilla de evaluación final fase 2
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACION FINAL FASE 2.xlsx
+++ b/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACION FINAL FASE 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://duoccl0-my.sharepoint.com/personal/ge_galan_profesor_duoc_cl/Documents/2024-2/Clases/CAPSTONE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="746" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A524BC42-4BE6-4992-8E50-65D453B1EC65}"/>
+  <xr:revisionPtr revIDLastSave="766" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FC3A1E2-2C9A-4A4B-8B7E-410474F053A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="78">
   <si>
     <t>Indicador de Evaluación</t>
   </si>
@@ -272,6 +272,12 @@
     <t>INDIVIDUAL</t>
   </si>
   <si>
+    <t>IGNACIO BELLO</t>
+  </si>
+  <si>
+    <t>LUCAS POBLETE</t>
+  </si>
+  <si>
     <t>Nivel de Logro</t>
   </si>
   <si>
@@ -288,6 +294,9 @@
   </si>
   <si>
     <t>Logro Incipiente</t>
+  </si>
+  <si>
+    <t>Logro incipiente</t>
   </si>
   <si>
     <t>Puntaje</t>
@@ -312,9 +321,6 @@
   </si>
   <si>
     <t>Relevancia</t>
-  </si>
-  <si>
-    <t>Logro incipiente</t>
   </si>
   <si>
     <t>Muy Relevante</t>
@@ -948,6 +954,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -957,20 +966,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -992,9 +1001,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,25 +1344,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="35" t="s">
@@ -1365,19 +1371,19 @@
       <c r="E2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="50"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="36">
         <v>-0.3</v>
       </c>
       <c r="E3" s="36">
         <v>0</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="55.15">
       <c r="A4" s="37" t="s">
@@ -1596,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K926"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1621,7 +1627,7 @@
       <c r="D2" s="2">
         <v>0.25</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="59">
         <v>1</v>
       </c>
     </row>
@@ -1635,24 +1641,26 @@
       <c r="D3" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="61"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="4" spans="1:11" ht="14.45">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="27" t="s">
+        <v>60</v>
+      </c>
       <c r="C4" s="5">
         <f>EVALUACION1!$C$21</f>
-        <v>7</v>
+        <v>3.3</v>
       </c>
       <c r="D4" s="5">
         <f>$C$32</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6">
         <f>C4*C$2+D4*D$2</f>
-        <v>7</v>
+        <v>3.4749999999999996</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1660,18 +1668,20 @@
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="27" t="s">
+        <v>61</v>
+      </c>
       <c r="C5" s="5">
         <f>EVALUACION1!$C$21</f>
-        <v>7</v>
+        <v>3.3</v>
       </c>
       <c r="D5" s="5">
         <f>C44</f>
-        <v>7</v>
+        <v>3.4</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
-        <v>7</v>
+        <v>3.3249999999999997</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1682,7 +1692,7 @@
       <c r="B6" s="27"/>
       <c r="C6" s="5">
         <f>EVALUACION1!$C$21</f>
-        <v>7</v>
+        <v>3.3</v>
       </c>
       <c r="D6" s="5">
         <f>C55</f>
@@ -1690,76 +1700,76 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4.2249999999999996</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="18" outlineLevel="1">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="60" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+        <v>62</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="1:11" ht="14.45" outlineLevel="1">
-      <c r="A12" s="64"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="56" t="s">
+      <c r="C12" s="62"/>
+      <c r="D12" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="55" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="64"/>
+      <c r="H12" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="64"/>
+      <c r="J12" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="63"/>
+      <c r="K12" s="64"/>
     </row>
     <row r="13" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A13" s="65"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="30" t="str">
         <f>RUBRICA!A4</f>
         <v>1. Implementa una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D13" s="16" t="str">
         <f t="shared" ref="D13:D16" si="1">IF($C13=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E13" s="16">
+        <v/>
+      </c>
+      <c r="E13" s="16" t="str">
         <f>IF(D13="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F13" s="16" t="str">
         <f t="shared" ref="F13:F16" si="2">IF($C13=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G13" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G13" s="16">
         <f>IF(F13="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H13" s="16" t="str">
         <f t="shared" ref="H13:H16" si="3">IF($C13=ML,"X","")</f>
@@ -1779,21 +1789,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="36" outlineLevel="1">
-      <c r="A14" s="65"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="30" t="str">
         <f>RUBRICA!A5</f>
         <v>2. Genera evidencias que dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D14" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E14" s="16">
+        <v/>
+      </c>
+      <c r="E14" s="16" t="str">
         <f>IF(D14="X",100*0.2,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="F14" s="16" t="str">
         <f t="shared" si="2"/>
@@ -1805,11 +1815,11 @@
       </c>
       <c r="H14" s="16" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I14" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="I14" s="16">
         <f>IF(H14="X",30*0.2,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="J14" s="16" t="str">
         <f t="shared" si="4"/>
@@ -1821,29 +1831,29 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A15" s="65"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="30" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Relaciona el Proyecto APT con las competencias del perfil de egreso de su Plan de Estudio.</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E15" s="16">
+        <v/>
+      </c>
+      <c r="E15" s="16" t="str">
         <f>IF(D15="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F15" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G15" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G15" s="16">
         <f>IF(F15="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H15" s="16" t="str">
         <f t="shared" si="3"/>
@@ -1863,29 +1873,29 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A16" s="65"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="30" t="str">
         <f>RUBRICA!A8</f>
         <v>5. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D16" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="E16" s="16">
+        <v/>
+      </c>
+      <c r="E16" s="16" t="str">
         <f>IF(D16="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F16" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G16" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G16" s="16">
         <f>IF(F16="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H16" s="16" t="str">
         <f t="shared" si="3"/>
@@ -1905,29 +1915,29 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A17" s="65"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="30" t="str">
         <f>RUBRICA!A9</f>
         <v xml:space="preserve">6. Utiliza correctamente las reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D17" s="16" t="str">
         <f>IF($C17=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E17" s="16">
+        <v/>
+      </c>
+      <c r="E17" s="16" t="str">
         <f>IF(D17="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F17" s="16" t="str">
         <f>IF($C17=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G17" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G17" s="16">
         <f>IF(F17="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H17" s="16" t="str">
         <f>IF($C17=ML,"X","")</f>
@@ -1947,21 +1957,21 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="24" outlineLevel="1">
-      <c r="A18" s="65"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="30" t="str">
         <f>RUBRICA!A10</f>
         <v>7. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D18" s="16" t="str">
         <f>IF($C18=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E18" s="16">
+        <v/>
+      </c>
+      <c r="E18" s="16" t="str">
         <f>IF(D18="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F18" s="16" t="str">
         <f>IF($C18=L,"X","")</f>
@@ -1973,11 +1983,11 @@
       </c>
       <c r="H18" s="16" t="str">
         <f>IF($C18=ML,"X","")</f>
-        <v/>
-      </c>
-      <c r="I18" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="I18" s="16">
         <f>IF(H18="X",30*0.15,"")</f>
-        <v/>
+        <v>4.5</v>
       </c>
       <c r="J18" s="16" t="str">
         <f>IF($C18=NL,"X","")</f>
@@ -1988,30 +1998,30 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22.9" customHeight="1" outlineLevel="1">
-      <c r="A19" s="65"/>
+    <row r="19" spans="1:11" ht="37.5" outlineLevel="1">
+      <c r="A19" s="66"/>
       <c r="B19" s="30" t="str">
         <f>RUBRICA!A12</f>
         <v>9.-Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D19" s="16" t="str">
         <f>IF($C19=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E19" s="16">
+        <v/>
+      </c>
+      <c r="E19" s="16" t="str">
         <f>IF(D19="X",100*0.15,"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="F19" s="16" t="str">
         <f>IF($C19=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G19" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G19" s="16">
         <f>IF(F19="X",60*0.15,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="H19" s="16" t="str">
         <f>IF($C19=ML,"X","")</f>
@@ -2031,28 +2041,28 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A20" s="64"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C20" s="33">
         <f>E20+G20+I20+K20</f>
-        <v>75</v>
+        <v>34.5</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19">
         <f>SUM(E13:E19)</f>
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19">
         <f>SUM(G13:G19)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19">
         <f>SUM(I13:I19)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19">
@@ -2061,13 +2071,13 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A21" s="61"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="32" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C21" s="20">
         <f>VLOOKUP(C20,ESCALA_IEP!A1:B152,2,FALSE)</f>
-        <v>7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1"/>
@@ -2076,101 +2086,101 @@
       <c r="A24" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="53">
+      <c r="B24" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="55" t="str">
         <f>$B$4</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="67"/>
+        <v>IGNACIO BELLO</v>
+      </c>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="64"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="70"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="64"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="63"/>
+        <v>62</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="64"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="64"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="63"/>
-      <c r="H27" s="56" t="s">
+      <c r="C27" s="62"/>
+      <c r="D27" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="63"/>
-      <c r="J27" s="55" t="s">
+      <c r="E27" s="64"/>
+      <c r="F27" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="64"/>
+      <c r="H27" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="64"/>
+      <c r="J27" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="63"/>
+      <c r="K27" s="64"/>
     </row>
     <row r="28" spans="1:11" ht="24">
-      <c r="A28" s="64"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="30" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D28" s="16" t="str">
         <f t="shared" ref="D28:D30" si="7">IF($C28=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E28" s="16">
+        <v/>
+      </c>
+      <c r="E28" s="16" t="str">
         <f>IF(D28="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F28" s="16" t="str">
         <f t="shared" ref="F28:F30" si="8">IF($C28=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G28" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G28" s="16">
         <f>IF(F28="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H28" s="16" t="str">
         <f t="shared" ref="H28:H30" si="9">IF($C28=ML,"X","")</f>
@@ -2190,29 +2200,29 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="24.6" customHeight="1">
-      <c r="A29" s="64"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="30" t="str">
         <f>RUBRICA!A11</f>
         <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D29" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="E29" s="16">
+        <v/>
+      </c>
+      <c r="E29" s="16" t="str">
         <f>IF(D29="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F29" s="16" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G29" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G29" s="16">
         <f>IF(F29="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H29" s="16" t="str">
         <f t="shared" si="9"/>
@@ -2232,29 +2242,29 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="25.9" customHeight="1">
-      <c r="A30" s="64"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="30" t="str">
         <f>RUBRICA!A13</f>
         <v>10. Colaboración y trabajo en equipo *</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D30" s="16" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="E30" s="16">
+        <v/>
+      </c>
+      <c r="E30" s="16" t="str">
         <f>IF(D30="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F30" s="16" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G30" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G30" s="16">
         <f>IF(F30="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H30" s="16" t="str">
         <f t="shared" si="9"/>
@@ -2274,23 +2284,23 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="64"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C31" s="18">
         <f>E31+G31+I31+K31</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19">
         <f>SUM(E28:E30)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19">
         <f>SUM(G28:G30)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="19">
@@ -2304,13 +2314,13 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="61"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C32" s="20">
         <f>VLOOKUP(C31,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
@@ -2326,101 +2336,101 @@
       <c r="A36" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="53">
+      <c r="B36" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="55" t="str">
         <f>B5</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="67"/>
+        <v>LUCAS POBLETE</v>
+      </c>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="68"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="64"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="70"/>
+      <c r="A37" s="65"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="64"/>
+      <c r="A38" s="65"/>
       <c r="B38" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="63"/>
+        <v>62</v>
+      </c>
+      <c r="D38" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="64"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="64"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="61"/>
-      <c r="D39" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="63"/>
-      <c r="H39" s="56" t="s">
+      <c r="C39" s="62"/>
+      <c r="D39" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="I39" s="63"/>
-      <c r="J39" s="55" t="s">
+      <c r="E39" s="64"/>
+      <c r="F39" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="64"/>
+      <c r="H39" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="64"/>
+      <c r="J39" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K39" s="63"/>
+      <c r="K39" s="64"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="64"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="30" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D40" s="16" t="str">
         <f t="shared" ref="D40:D42" si="12">IF($C40=CL,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="E40" s="16">
+        <v/>
+      </c>
+      <c r="E40" s="16" t="str">
         <f>IF(D40="X",100*0.05,"")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F40" s="16" t="str">
         <f t="shared" ref="F40:F42" si="13">IF($C40=L,"X","")</f>
-        <v/>
-      </c>
-      <c r="G40" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G40" s="16">
         <f>IF(F40="X",60*0.05,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H40" s="16" t="str">
         <f t="shared" ref="H40:H42" si="14">IF($C40=ML,"X","")</f>
@@ -2440,21 +2450,21 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="25.9" customHeight="1">
-      <c r="A41" s="64"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="30" t="str">
         <f>RUBRICA!A11</f>
         <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D41" s="16" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="E41" s="16">
+        <v/>
+      </c>
+      <c r="E41" s="16" t="str">
         <f>IF(D41="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F41" s="16" t="str">
         <f t="shared" si="13"/>
@@ -2466,11 +2476,11 @@
       </c>
       <c r="H41" s="16" t="str">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="I41" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="I41" s="16">
         <f>IF(H41="X",30*0.1,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="J41" s="16" t="str">
         <f t="shared" si="15"/>
@@ -2482,29 +2492,29 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="14.45">
-      <c r="A42" s="64"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="30" t="str">
         <f>RUBRICA!A13</f>
         <v>10. Colaboración y trabajo en equipo *</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D42" s="16" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="E42" s="16">
+        <v/>
+      </c>
+      <c r="E42" s="16" t="str">
         <f>IF(D42="X",100*0.1,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="F42" s="16" t="str">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G42" s="16" t="str">
+        <v>X</v>
+      </c>
+      <c r="G42" s="16">
         <f>IF(F42="X",60*0.1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="H42" s="16" t="str">
         <f t="shared" si="14"/>
@@ -2524,28 +2534,28 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="64"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C43" s="18">
         <f>E43+G43+I43+K43</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19">
         <f>SUM(E40:E42)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19">
         <f>SUM(G40:G42)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="19">
         <f>SUM(I40:I42)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J43" s="19"/>
       <c r="K43" s="19">
@@ -2554,13 +2564,13 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="61"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C44" s="20">
         <f>VLOOKUP(C43,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
-        <v>7</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
@@ -2575,85 +2585,85 @@
       <c r="A47" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="53">
+      <c r="B47" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="55">
         <f>B6</f>
         <v>0</v>
       </c>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="66"/>
-      <c r="G47" s="66"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="68"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A48" s="64"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="69"/>
-      <c r="J48" s="69"/>
-      <c r="K48" s="70"/>
+      <c r="A48" s="65"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+      <c r="K48" s="71"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A49" s="64"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="63"/>
+        <v>62</v>
+      </c>
+      <c r="D49" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="K49" s="64"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A50" s="64"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="E50" s="63"/>
-      <c r="F50" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G50" s="63"/>
-      <c r="H50" s="56" t="s">
+      <c r="C50" s="62"/>
+      <c r="D50" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="I50" s="63"/>
-      <c r="J50" s="55" t="s">
+      <c r="E50" s="64"/>
+      <c r="F50" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="64"/>
+      <c r="H50" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="I50" s="64"/>
+      <c r="J50" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K50" s="63"/>
+      <c r="K50" s="64"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A51" s="64"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="30" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D51" s="16" t="str">
         <f t="shared" ref="D51:D53" si="17">IF($C51=CL,"X","")</f>
@@ -2689,13 +2699,13 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="25.9" customHeight="1">
-      <c r="A52" s="64"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="30" t="str">
         <f>RUBRICA!A11</f>
         <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D52" s="16" t="str">
         <f t="shared" si="17"/>
@@ -2731,13 +2741,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.45">
-      <c r="A53" s="64"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="30" t="str">
         <f>RUBRICA!A13</f>
         <v>10. Colaboración y trabajo en equipo *</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D53" s="16" t="str">
         <f t="shared" si="17"/>
@@ -2773,9 +2783,9 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A54" s="64"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C54" s="18">
         <f>E54+G54+I54+K54</f>
@@ -2803,9 +2813,9 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A55" s="61"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C55" s="20">
         <f>VLOOKUP(C54,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
@@ -3688,17 +3698,14 @@
     <row r="926" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C47:K48"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:K37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
     <mergeCell ref="A36:A44"/>
     <mergeCell ref="A24:A32"/>
     <mergeCell ref="E2:E3"/>
@@ -3715,14 +3722,17 @@
     <mergeCell ref="D26:K26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:K37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C47:K48"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -3747,7 +3757,7 @@
           <x14:formula1>
             <xm:f>'RELEVANCIA-PUNTAJE'!$B$2:$E$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C40:C42 C13:C19 C28:C30 C51:C53</xm:sqref>
+          <xm:sqref>C13:C19 C51:C53 C28:C30 C40:C42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3770,10 +3780,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.45">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45">
@@ -5851,10 +5861,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.45">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45">
@@ -7248,10 +7258,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.45">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45">
@@ -8634,34 +8644,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45">
-      <c r="A1" s="60" t="s">
-        <v>73</v>
+      <c r="A1" s="61" t="s">
+        <v>76</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="43.9" thickBot="1">
-      <c r="A2" s="71"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.45" thickBot="1">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" s="13">
         <v>4</v>

</xml_diff>